<commit_message>
Noted all channel behaviour for August
</commit_message>
<xml_diff>
--- a/CIS Updates/Odd Channel Behavior.xlsx
+++ b/CIS Updates/Odd Channel Behavior.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\CIS Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931CDB80-1A9F-42F7-991E-0108EA4DB20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B074BA2E-C6E8-4C4B-8825-9B10C72186B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8E44477-D6C0-4A59-A814-E37C4647FF29}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>EBA</t>
   </si>
@@ -243,6 +243,138 @@
   </si>
   <si>
     <t>weird step. (recal)</t>
+  </si>
+  <si>
+    <t>Unusually low CIS constant, some high schatter near end of month, ADC masked</t>
+  </si>
+  <si>
+    <t>Half gain (not in update)</t>
+  </si>
+  <si>
+    <t>EBA_m19_c41_highgain</t>
+  </si>
+  <si>
+    <t>Drift at end of month, see if it continues (not in update)</t>
+  </si>
+  <si>
+    <t>Very frar from detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Unusually low constant, ADC affected (not in update)</t>
+  </si>
+  <si>
+    <t>Unusually low compared to detecto average, ADC affected (not in update)</t>
+  </si>
+  <si>
+    <t>Half gain (not in update), ADC masked</t>
+  </si>
+  <si>
+    <t>High scatter</t>
+  </si>
+  <si>
+    <t>Upwards drift, unusually far from detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Very high scatter,no discernable trend, severe stuck bit</t>
+  </si>
+  <si>
+    <t>Much lower than detector average</t>
+  </si>
+  <si>
+    <t>Much lower than detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Not exactly half gain channel - something else? High scatter. (not in update). DEFAULT (masked)</t>
+  </si>
+  <si>
+    <t>EBC_m30_c11_highgain</t>
+  </si>
+  <si>
+    <t>High scatter at the end of the month</t>
+  </si>
+  <si>
+    <t>EBC_m30_c11_lowgain</t>
+  </si>
+  <si>
+    <t>Very far from detector average (not in update)</t>
+  </si>
+  <si>
+    <t>Drifting downwards, away from detector average</t>
+  </si>
+  <si>
+    <t>Very far from detector average</t>
+  </si>
+  <si>
+    <t>LBA_m02_c06_highgain</t>
+  </si>
+  <si>
+    <t>Slight downward drift, noticeable step near end (not in update)</t>
+  </si>
+  <si>
+    <t>LBA_m02_c06_lowgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very far from detector average, larga scatter getting worse at end of time interval </t>
+  </si>
+  <si>
+    <t>LBA_m52_c01_lowgain</t>
+  </si>
+  <si>
+    <t>Add bad CIS?</t>
+  </si>
+  <si>
+    <t>DEFAULT (not in update)</t>
+  </si>
+  <si>
+    <t>Very far from detector average, drift at end of month with high scatter (not in update)</t>
+  </si>
+  <si>
+    <t>LBC_m10_c37_highgain</t>
+  </si>
+  <si>
+    <t>Remove bad CIS?</t>
+  </si>
+  <si>
+    <t>LBC_m13_c15_highgain</t>
+  </si>
+  <si>
+    <t>LBC_m13_c15_lowgain</t>
+  </si>
+  <si>
+    <t>Recalibrate from the end of July (not in update)</t>
+  </si>
+  <si>
+    <t>Drifting up, hige step and scatter</t>
+  </si>
+  <si>
+    <t>Large scatter (40% RMS/mean), ADC masked</t>
+  </si>
+  <si>
+    <t>Very high scatter</t>
+  </si>
+  <si>
+    <t>Step jump in middle, still high scatter after the jump, so recalibration would not help</t>
+  </si>
+  <si>
+    <t>Realibrate to middle of month? Step jump in middle, still slight scatter after the jump,</t>
+  </si>
+  <si>
+    <t>LBC_m44_c35_highgain</t>
+  </si>
+  <si>
+    <t>Add bad CIS? It's drifting downwards</t>
+  </si>
+  <si>
+    <t>High scatter in middle of month</t>
+  </si>
+  <si>
+    <t>Far from detector average, high scatter, channel masked anyways</t>
+  </si>
+  <si>
+    <t>LBC_m63_c45_highgain</t>
+  </si>
+  <si>
+    <t>Remove bad CIS?  (not in update)</t>
   </si>
 </sst>
 </file>
@@ -271,7 +403,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +419,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -347,6 +497,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0386BC-E96B-43FA-B2D4-F7AC885F6095}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,161 +870,359 @@
       </c>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+    <row r="2" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+    <row r="3" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+    <row r="4" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="F4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+    <row r="5" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>101</v>
+      </c>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
+    <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="F6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>102</v>
+      </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+    <row r="7" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+    <row r="8" spans="1:10" ht="53.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+    <row r="9" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+    <row r="10" spans="1:10" ht="66.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+    <row r="11" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+    <row r="12" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
+      <c r="H12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>108</v>
+      </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
+      <c r="H13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>